<commit_message>
Renamed parameter => name
</commit_message>
<xml_diff>
--- a/util/metadata1.xlsx
+++ b/util/metadata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="33200" yWindow="-740" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="1100" yWindow="0" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sect1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>is_primary</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>py_type</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -485,7 +488,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
generating params.py, but without docstring
</commit_message>
<xml_diff>
--- a/util/metadata1.xlsx
+++ b/util/metadata1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="0" windowWidth="25040" windowHeight="17000" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="21160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="sect1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
   <si>
     <t>is_primary</t>
   </si>
@@ -28,9 +28,6 @@
     <t>units</t>
   </si>
   <si>
-    <t>parameter</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -43,18 +40,9 @@
     <t>m</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>int_in</t>
   </si>
   <si>
-    <t>float_m</t>
-  </si>
-  <si>
-    <t xml:space="preserve">a floating point measure of meters </t>
-  </si>
-  <si>
     <t>an integer measuring inches</t>
   </si>
   <si>
@@ -83,6 +71,39 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>sect2 desc here</t>
+  </si>
+  <si>
+    <t>sect1 desc</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t xml:space="preserve">μMeter: floating point measure of meters </t>
+  </si>
+  <si>
+    <t>float_um</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>unicode_value</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>hêllö</t>
+  </si>
+  <si>
+    <t>String with unicode default value</t>
   </si>
 </sst>
 </file>
@@ -95,6 +116,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -131,21 +153,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,80 +504,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="49.33203125" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -564,66 +627,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="5" max="5" width="62.1640625" customWidth="1"/>
+    <col min="6" max="6" width="62.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>-1.3</v>
+      </c>
+      <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
major refactoring so clearer code. Still need to generate autodoc
</commit_message>
<xml_diff>
--- a/util/metadata1.xlsx
+++ b/util/metadata1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="17560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sect1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>is_primary</t>
   </si>
@@ -70,24 +70,15 @@
     <t>py_type</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>sect2 desc here</t>
   </si>
   <si>
-    <t>sect1 desc</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
     <t>False</t>
   </si>
   <si>
-    <t xml:space="preserve">μMeter: floating point measure of meters </t>
-  </si>
-  <si>
     <t>float_um</t>
   </si>
   <si>
@@ -104,6 +95,27 @@
   </si>
   <si>
     <t>String with unicode default value</t>
+  </si>
+  <si>
+    <t>py_name</t>
+  </si>
+  <si>
+    <t>display_name</t>
+  </si>
+  <si>
+    <t>arPrecF[1]</t>
+  </si>
+  <si>
+    <t>arPrecF[0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">floating point measure of meters </t>
+  </si>
+  <si>
+    <t>μMeter</t>
+  </si>
+  <si>
+    <t>sect1 description</t>
   </si>
 </sst>
 </file>
@@ -504,114 +516,118 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="49.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -627,79 +643,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="62.1640625" customWidth="1"/>
+    <col min="7" max="7" width="62.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-1.3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>